<commit_message>
Added Obstacles 5x4 grid
Added alternative Obstacles sheet with a 5x4 grid for holding 35x48mm Post-it notes.
You can prioritize or group together related obstacles in different rows and columns. 
There is a placeholder box to hold the one obstacle that you are working on now. It's only big enough to hold one sticker!
</commit_message>
<xml_diff>
--- a/StoryboardSheets.xlsx
+++ b/StoryboardSheets.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devschool\Improvement Kata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Internal\dfs$\MEL-EXTENDED_MOEUSERLIBRARIES\mjones\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27636" windowHeight="7968" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Obstacles" sheetId="5" r:id="rId1"/>
-    <sheet name="Target" sheetId="6" r:id="rId2"/>
-    <sheet name="Current" sheetId="8" r:id="rId3"/>
+    <sheet name="Obstacle 5x4" sheetId="10" r:id="rId1"/>
+    <sheet name="Obstacles" sheetId="5" r:id="rId2"/>
+    <sheet name="Target" sheetId="6" r:id="rId3"/>
+    <sheet name="Current" sheetId="8" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Obstacles!$A:$B</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Process Metric</t>
   </si>
@@ -65,13 +69,20 @@
   </si>
   <si>
     <t xml:space="preserve">Metrics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which ONE obstacle are you addressing now?  ---&gt;  </t>
+  </si>
+  <si>
+    <t>Stick a 35 x 48 mm 
+Post-It note here!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +111,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -198,16 +223,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -223,15 +260,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -257,8 +285,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,147 +624,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="136.85546875" customWidth="1"/>
+    <col min="1" max="5" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" s="20" customFormat="1" ht="106.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="133.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="252" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="252" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="184.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -725,110 +857,110 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
-    <col min="3" max="12" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="12" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-    </row>
-    <row r="2" spans="1:12" s="15" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:12" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" s="15" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" s="15" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+    </row>
+    <row r="3" spans="1:12" s="11" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" s="11" customFormat="1" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
-    </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -843,133 +975,165 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" spans="1:12" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
         <v>4</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>7</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -978,7 +1142,7 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>